<commit_message>
created script and data to load keywords and types
</commit_message>
<xml_diff>
--- a/data/keywords_and_types.xlsx
+++ b/data/keywords_and_types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38D85BA4-8DEC-9641-AA99-079F7494CD15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83519933-B3D9-F840-8DFF-4EE4CF4725F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Image types" sheetId="3" r:id="rId3"/>
     <sheet name="Text types" sheetId="5" r:id="rId4"/>
     <sheet name="PictureStory types" sheetId="7" r:id="rId5"/>
-    <sheet name="Infographics types" sheetId="6" r:id="rId6"/>
+    <sheet name="Infographic types" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="199">
   <si>
     <t>We envision these as overarching keywords, with nested further definitions (so, for example, 'people' further categorises into 'women'.
 Ideally, this would also be the way in which end users can then search by category through the materials.</t>
@@ -516,9 +516,6 @@
     <t>recipes</t>
   </si>
   <si>
-    <t>fiction</t>
-  </si>
-  <si>
     <t>poetry</t>
   </si>
   <si>
@@ -529,9 +526,6 @@
   </si>
   <si>
     <t>drama</t>
-  </si>
-  <si>
-    <t>non-fiction</t>
   </si>
   <si>
     <t>quotes</t>
@@ -1168,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -1186,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C1" s="49" t="s">
         <v>1</v>
@@ -1391,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D23" s="33"/>
     </row>
@@ -1537,7 +1531,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>12</v>
@@ -1809,7 +1803,7 @@
         <v>21</v>
       </c>
       <c r="C69" s="41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D69" s="27"/>
     </row>
@@ -2362,7 +2356,7 @@
         <v>68</v>
       </c>
       <c r="C130" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D130" s="27"/>
     </row>
@@ -2404,7 +2398,7 @@
     </row>
     <row r="135" spans="2:4" ht="15.75" customHeight="1">
       <c r="B135" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>142</v>
@@ -2413,7 +2407,7 @@
     </row>
     <row r="136" spans="2:4" ht="15.75" customHeight="1">
       <c r="B136" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C136" s="40" t="s">
         <v>143</v>
@@ -2422,28 +2416,28 @@
     </row>
     <row r="137" spans="2:4" ht="15.75" customHeight="1">
       <c r="B137" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C137" s="40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D137" s="27"/>
     </row>
     <row r="138" spans="2:4" ht="15.75" customHeight="1">
       <c r="B138" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C138" s="40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D138" s="27"/>
     </row>
     <row r="139" spans="2:4" ht="15.75" customHeight="1">
       <c r="B139" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C139" s="40" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D139" s="27"/>
     </row>
@@ -5184,17 +5178,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -5219,42 +5213,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -5264,10 +5258,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC4CA93-A9C4-4E0D-A378-CAF06948FED3}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5276,170 +5270,144 @@
     <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="B23" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="B26" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="B27" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="B28" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -5459,22 +5427,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -5494,17 +5462,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>